<commit_message>
incorporar a main la nueva variable activa, no estaba en la clase de gestoría
</commit_message>
<xml_diff>
--- a/POST/plantilla_gestorias.xlsx
+++ b/POST/plantilla_gestorias.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emilio Hurtado\Desktop\taxrating\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC1C5EB-DA84-4E3E-8E82-09555346D4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Nombre</t>
   </si>
@@ -28,12 +22,18 @@
     <t>Imagen</t>
   </si>
   <si>
+    <t>Web</t>
+  </si>
+  <si>
     <t>Ubicación</t>
   </si>
   <si>
     <t>Provincia</t>
   </si>
   <si>
+    <t>Valoraciones</t>
+  </si>
+  <si>
     <t>Valoración Global</t>
   </si>
   <si>
@@ -52,6 +52,9 @@
     <t>Asesoría Internacional</t>
   </si>
   <si>
+    <t>Activa</t>
+  </si>
+  <si>
     <t>Asesoría Contable S.L.</t>
   </si>
   <si>
@@ -61,12 +64,36 @@
     <t>Consultoría Fiscal ABC</t>
   </si>
   <si>
+    <t>Justo Gallardo Asesores</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/1447567421/es/foto/joven-empresaria-feliz-teniendo-una-reuni%C3%B3n-con-sus-colegas-en-la-oficina-y-mirando-a-la-c%C3%A1mara.jpg?s=612x612&amp;w=0&amp;k=20&amp;c=h_vuWKesK85NkJr_zI9L9AhD3yXiuZzqzMQi1e1Nsv0=</t>
+  </si>
+  <si>
+    <t>https://media.gettyimages.com/id/1147479610/es/foto/la-toma-de-decisiones-es-mejor-cuando-lo-haces-juntos.jpg?s=612x612&amp;w=gi&amp;k=20&amp;c=nA5y9HmOG8RuFwa1LLukYvnuNo79pByHCriTmDLK2Fo=</t>
+  </si>
+  <si>
+    <t>https://gestoriagabaldon.com/wp-content/uploads/2019/02/logo_gac.png</t>
+  </si>
+  <si>
+    <t>https://gestoriamadrid.com</t>
+  </si>
+  <si>
+    <t>https://justogallardoasesores.com/</t>
+  </si>
+  <si>
     <t>https://maps.google.com/?q=Asesoría+Contable+S.L.</t>
   </si>
   <si>
     <t>https://maps.google.com/?q=Gestoría+Pérez+y+Asociados</t>
   </si>
   <si>
+    <t>https://maps.app.goo.gl/vRe8kdBvrpwrBL636</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/JtZpa56X49fiEfH56</t>
+  </si>
+  <si>
     <t>Madrid</t>
   </si>
   <si>
@@ -76,44 +103,14 @@
     <t>Valencia</t>
   </si>
   <si>
-    <t>https://maps.app.goo.gl/vRe8kdBvrpwrBL636</t>
-  </si>
-  <si>
-    <t>https://media.istockphoto.com/id/1447567421/es/foto/joven-empresaria-feliz-teniendo-una-reuni%C3%B3n-con-sus-colegas-en-la-oficina-y-mirando-a-la-c%C3%A1mara.jpg?s=612x612&amp;w=0&amp;k=20&amp;c=h_vuWKesK85NkJr_zI9L9AhD3yXiuZzqzMQi1e1Nsv0=</t>
-  </si>
-  <si>
-    <t>https://media.gettyimages.com/id/1147479610/es/foto/la-toma-de-decisiones-es-mejor-cuando-lo-haces-juntos.jpg?s=612x612&amp;w=gi&amp;k=20&amp;c=nA5y9HmOG8RuFwa1LLukYvnuNo79pByHCriTmDLK2Fo=</t>
-  </si>
-  <si>
-    <t>https://gestoriagabaldon.com/wp-content/uploads/2019/02/logo_gac.png</t>
-  </si>
-  <si>
     <t>Badajoz</t>
-  </si>
-  <si>
-    <t>https://gestoriamadrid.com</t>
-  </si>
-  <si>
-    <t>Web</t>
-  </si>
-  <si>
-    <t>https://justogallardoasesores.com/</t>
-  </si>
-  <si>
-    <t>Justo Gallardo Asesores</t>
-  </si>
-  <si>
-    <t>https://maps.app.goo.gl/JtZpa56X49fiEfH56</t>
-  </si>
-  <si>
-    <t>Valoraciones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,26 +181,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -241,7 +230,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -275,7 +264,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -310,10 +298,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -486,19 +473,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="3" width="22.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,71 +488,76 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2">
-        <v>10</v>
-      </c>
       <c r="G3">
-        <f>AVERAGE(H3:L3)</f>
         <v>3.16</v>
       </c>
       <c r="H3">
@@ -583,24 +570,27 @@
         <v>4.3</v>
       </c>
       <c r="K3">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="L3">
         <v>2.4</v>
       </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F4">
         <v>20</v>
@@ -609,62 +599,71 @@
         <v>4.8</v>
       </c>
       <c r="H4">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="J4">
         <v>4.7</v>
       </c>
       <c r="K4">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="L4">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="2">
+        <v>29</v>
+      </c>
+      <c r="F5">
         <v>65</v>
       </c>
       <c r="G5">
         <v>4.8</v>
       </c>
       <c r="H5">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="J5">
         <v>4.7</v>
       </c>
       <c r="K5">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="L5">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E7" s="2"/>
-      <c r="G7" s="2"/>
+        <v>4.4</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId8"/>
+    <hyperlink ref="C5" r:id="rId9"/>
+    <hyperlink ref="D5" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modificar desplegable de servicios valorados
</commit_message>
<xml_diff>
--- a/POST/plantilla_gestorias.xlsx
+++ b/POST/plantilla_gestorias.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\taxrating\POST\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E25D141-82FF-49B9-A11F-7BE9B950FBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Nombre</t>
   </si>
@@ -116,13 +122,22 @@
   </si>
   <si>
     <t>test@example.com</t>
+  </si>
+  <si>
+    <t>00000002T</t>
+  </si>
+  <si>
+    <t>00000003T</t>
+  </si>
+  <si>
+    <t>00000004T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,18 +208,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -242,7 +265,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -276,6 +299,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -310,9 +334,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,14 +510,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="23.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -562,7 +593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -594,22 +625,22 @@
         <v>4.3</v>
       </c>
       <c r="K3">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="L3">
         <v>2.4</v>
       </c>
       <c r="M3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -629,28 +660,28 @@
         <v>4.8</v>
       </c>
       <c r="H4">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="J4">
         <v>4.7</v>
       </c>
       <c r="K4">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="L4">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="O4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -673,22 +704,22 @@
         <v>4.8</v>
       </c>
       <c r="H5">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="J5">
         <v>4.7</v>
       </c>
       <c r="K5">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="L5">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="O5" t="s">
         <v>33</v>
@@ -696,16 +727,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="D4" r:id="rId7"/>
-    <hyperlink ref="B5" r:id="rId8"/>
-    <hyperlink ref="C5" r:id="rId9"/>
-    <hyperlink ref="D5" r:id="rId10"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D5" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>